<commit_message>
Added some requirements, first use case.
</commit_message>
<xml_diff>
--- a/Functional Requirements.xlsx
+++ b/Functional Requirements.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17329"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -11,12 +11,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
   <si>
     <t>ID</t>
   </si>
@@ -39,15 +39,9 @@
     <t>Status</t>
   </si>
   <si>
-    <t>Represantation of text for reading</t>
-  </si>
-  <si>
     <t>Texts could be heared as audio</t>
   </si>
   <si>
-    <t>Selected sub-texts could be heared as audio</t>
-  </si>
-  <si>
     <t>Representation of definitions of difficult words</t>
   </si>
   <si>
@@ -69,12 +63,6 @@
     <t>Feedback for repeated words in an answer</t>
   </si>
   <si>
-    <t>Suggestions of alternative for repeated words</t>
-  </si>
-  <si>
-    <t>Hyper links to external educational online games</t>
-  </si>
-  <si>
     <t>Score accumulatation for external educational online games</t>
   </si>
   <si>
@@ -169,13 +157,40 @@
   </si>
   <si>
     <t>Existing teachers could be appointed as admins</t>
+  </si>
+  <si>
+    <t>Representation of text for reading</t>
+  </si>
+  <si>
+    <t>Selected sub-texts could be heard as audio</t>
+  </si>
+  <si>
+    <t>Suggestions of alternatives for repeated words in an answer</t>
+  </si>
+  <si>
+    <t>Hyperlinks to external educational online games</t>
+  </si>
+  <si>
+    <t>new ones</t>
+  </si>
+  <si>
+    <t>Pupils could log in to the system</t>
+  </si>
+  <si>
+    <t>Pupils could log out of the system</t>
+  </si>
+  <si>
+    <t>Teachers could log in to the system</t>
+  </si>
+  <si>
+    <t>Teachers could log out of the system</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -212,7 +227,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -220,12 +235,22 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -272,7 +297,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -304,9 +329,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -338,6 +381,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -513,14 +574,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="52" customWidth="1"/>
     <col min="4" max="4" width="11.625" customWidth="1"/>
@@ -529,7 +590,7 @@
     <col min="7" max="7" width="16.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15">
+    <row r="1" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -552,386 +613,623 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
+        <v>47</v>
+      </c>
+      <c r="C2">
+        <v>5</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="E2" s="3">
+        <v>42686</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
+        <v>7</v>
+      </c>
+      <c r="C3">
+        <v>4</v>
+      </c>
+      <c r="D3">
+        <v>4</v>
+      </c>
+      <c r="E3" s="3">
+        <v>42686</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
+        <v>48</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>5</v>
+      </c>
+      <c r="E4" s="3">
+        <v>42686</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
+        <v>8</v>
+      </c>
+      <c r="C5">
+        <v>5</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5" s="3">
+        <v>42686</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
+        <v>9</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+      <c r="D6">
+        <v>3</v>
+      </c>
+      <c r="E6" s="3">
+        <v>42686</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
+        <v>10</v>
+      </c>
+      <c r="C7">
+        <v>5</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7" s="3">
+        <v>42686</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
+        <v>11</v>
+      </c>
+      <c r="C8">
+        <v>5</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8" s="3">
+        <v>42686</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
+        <v>12</v>
+      </c>
+      <c r="C9">
+        <v>5</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9" s="3">
+        <v>42686</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
+        <v>13</v>
+      </c>
+      <c r="C10">
+        <v>5</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10" s="3">
+        <v>42686</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
+        <v>14</v>
+      </c>
+      <c r="C11">
+        <v>5</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11" s="3">
+        <v>42686</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
+        <v>49</v>
+      </c>
+      <c r="C12">
+        <v>4</v>
+      </c>
+      <c r="D12">
+        <v>3</v>
+      </c>
+      <c r="E12" s="3">
+        <v>42686</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
+        <v>50</v>
+      </c>
+      <c r="C13">
+        <v>4</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13" s="3">
+        <v>42686</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
+        <v>15</v>
+      </c>
+      <c r="C14">
+        <v>3</v>
+      </c>
+      <c r="D14">
+        <v>5</v>
+      </c>
+      <c r="E14" s="3">
+        <v>42686</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
+        <v>16</v>
+      </c>
+      <c r="C15">
+        <v>3</v>
+      </c>
+      <c r="D15">
+        <v>5</v>
+      </c>
+      <c r="E15" s="3">
+        <v>42686</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
+        <v>17</v>
+      </c>
+      <c r="C16">
+        <v>4</v>
+      </c>
+      <c r="D16">
+        <v>4</v>
+      </c>
+      <c r="E16" s="3">
+        <v>42686</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
+        <v>18</v>
+      </c>
+      <c r="E17" s="3">
+        <v>42686</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
+        <v>19</v>
+      </c>
+      <c r="E18" s="3">
+        <v>42686</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
+        <v>20</v>
+      </c>
+      <c r="E19" s="3">
+        <v>42686</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
+        <v>21</v>
+      </c>
+      <c r="E20" s="3">
+        <v>42686</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
+        <v>22</v>
+      </c>
+      <c r="E21" s="3">
+        <v>42686</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2">
+        <v>25</v>
+      </c>
+      <c r="E22" s="3">
+        <v>42686</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2">
+        <v>23</v>
+      </c>
+      <c r="E23" s="3">
+        <v>42686</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2">
+        <v>24</v>
+      </c>
+      <c r="E24" s="3">
+        <v>42686</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2">
+        <v>26</v>
+      </c>
+      <c r="E25" s="3">
+        <v>42686</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2">
+        <v>27</v>
+      </c>
+      <c r="E26" s="3">
+        <v>42686</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2">
+        <v>28</v>
+      </c>
+      <c r="E27" s="3">
+        <v>42686</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2">
+        <v>29</v>
+      </c>
+      <c r="E28" s="3">
+        <v>42686</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2">
+        <v>30</v>
+      </c>
+      <c r="E29" s="3">
+        <v>42686</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2">
+        <v>31</v>
+      </c>
+      <c r="E30" s="3">
+        <v>42686</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2">
+        <v>32</v>
+      </c>
+      <c r="E31" s="3">
+        <v>42686</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2">
+        <v>33</v>
+      </c>
+      <c r="E32" s="3">
+        <v>42686</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2">
+        <v>34</v>
+      </c>
+      <c r="E33" s="3">
+        <v>42686</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2">
+        <v>35</v>
+      </c>
+      <c r="E34" s="3">
+        <v>42686</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2">
+        <v>36</v>
+      </c>
+      <c r="E35" s="3">
+        <v>42686</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2">
+        <v>37</v>
+      </c>
+      <c r="E36" s="3">
+        <v>42686</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2">
+        <v>38</v>
+      </c>
+      <c r="E37" s="3">
+        <v>42686</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2">
+        <v>39</v>
+      </c>
+      <c r="E38" s="3">
+        <v>42686</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2">
+        <v>40</v>
+      </c>
+      <c r="E39" s="3">
+        <v>42686</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2">
+        <v>41</v>
+      </c>
+      <c r="E40" s="3">
+        <v>42686</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2">
+        <v>42</v>
+      </c>
+      <c r="E41" s="3">
+        <v>42686</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2">
+        <v>43</v>
+      </c>
+      <c r="E42" s="3">
+        <v>42686</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2">
+        <v>44</v>
+      </c>
+      <c r="E43" s="3">
+        <v>42686</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2">
+        <v>46</v>
+      </c>
+      <c r="E44" s="3">
+        <v>42686</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2">
+        <v>45</v>
+      </c>
+      <c r="E45" s="3">
+        <v>42686</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:2">
+    <row r="47" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>46</v>
       </c>
-    </row>
-    <row r="48" spans="1:2">
+      <c r="B47" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>47</v>
       </c>
-    </row>
-    <row r="49" spans="1:1">
+      <c r="B48" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>48</v>
       </c>
-    </row>
-    <row r="50" spans="1:1">
+      <c r="B49" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>49</v>
       </c>
-    </row>
-    <row r="51" spans="1:1">
+      <c r="B50" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>50</v>
+      </c>
+      <c r="B51" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -941,26 +1239,26 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
7 use cases added
</commit_message>
<xml_diff>
--- a/Functional Requirements.xlsx
+++ b/Functional Requirements.xlsx
@@ -39,12 +39,6 @@
     <t>Status</t>
   </si>
   <si>
-    <t>Texts could be heared as audio</t>
-  </si>
-  <si>
-    <t>Representation of definitions of difficult words</t>
-  </si>
-  <si>
     <t>Ability to answer questions related to a text</t>
   </si>
   <si>
@@ -159,9 +153,6 @@
     <t>Existing teachers could be appointed as admins</t>
   </si>
   <si>
-    <t>Representation of text for reading</t>
-  </si>
-  <si>
     <t>Selected sub-texts could be heard as audio</t>
   </si>
   <si>
@@ -184,6 +175,15 @@
   </si>
   <si>
     <t>Teachers could log out of the system</t>
+  </si>
+  <si>
+    <t>Texts could be heard as audio</t>
+  </si>
+  <si>
+    <t>Viewing definitions of difficult words</t>
+  </si>
+  <si>
+    <t>Viewing text for reading</t>
   </si>
 </sst>
 </file>
@@ -577,8 +577,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B47" sqref="B47"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -618,7 +618,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="C2">
         <v>5</v>
@@ -635,7 +635,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>53</v>
       </c>
       <c r="C3">
         <v>4</v>
@@ -652,7 +652,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -669,7 +669,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>54</v>
       </c>
       <c r="C5">
         <v>5</v>
@@ -686,7 +686,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C6">
         <v>5</v>
@@ -703,7 +703,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C7">
         <v>5</v>
@@ -720,7 +720,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C8">
         <v>5</v>
@@ -737,7 +737,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C9">
         <v>5</v>
@@ -754,7 +754,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C10">
         <v>5</v>
@@ -771,7 +771,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C11">
         <v>5</v>
@@ -788,7 +788,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C12">
         <v>4</v>
@@ -805,7 +805,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C13">
         <v>4</v>
@@ -822,7 +822,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C14">
         <v>3</v>
@@ -839,7 +839,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C15">
         <v>3</v>
@@ -856,7 +856,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C16">
         <v>4</v>
@@ -873,7 +873,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E17" s="3">
         <v>42686</v>
@@ -884,7 +884,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E18" s="3">
         <v>42686</v>
@@ -895,7 +895,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E19" s="3">
         <v>42686</v>
@@ -906,7 +906,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E20" s="3">
         <v>42686</v>
@@ -917,7 +917,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E21" s="3">
         <v>42686</v>
@@ -928,7 +928,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E22" s="3">
         <v>42686</v>
@@ -939,7 +939,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E23" s="3">
         <v>42686</v>
@@ -950,7 +950,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E24" s="3">
         <v>42686</v>
@@ -961,7 +961,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E25" s="3">
         <v>42686</v>
@@ -972,7 +972,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E26" s="3">
         <v>42686</v>
@@ -983,7 +983,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E27" s="3">
         <v>42686</v>
@@ -994,7 +994,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E28" s="3">
         <v>42686</v>
@@ -1005,7 +1005,7 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E29" s="3">
         <v>42686</v>
@@ -1016,7 +1016,7 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E30" s="3">
         <v>42686</v>
@@ -1027,7 +1027,7 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E31" s="3">
         <v>42686</v>
@@ -1038,7 +1038,7 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E32" s="3">
         <v>42686</v>
@@ -1049,7 +1049,7 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E33" s="3">
         <v>42686</v>
@@ -1060,7 +1060,7 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E34" s="3">
         <v>42686</v>
@@ -1071,7 +1071,7 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E35" s="3">
         <v>42686</v>
@@ -1082,7 +1082,7 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E36" s="3">
         <v>42686</v>
@@ -1093,7 +1093,7 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E37" s="3">
         <v>42686</v>
@@ -1104,7 +1104,7 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E38" s="3">
         <v>42686</v>
@@ -1115,7 +1115,7 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E39" s="3">
         <v>42686</v>
@@ -1126,7 +1126,7 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E40" s="3">
         <v>42686</v>
@@ -1137,7 +1137,7 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E41" s="3">
         <v>42686</v>
@@ -1148,7 +1148,7 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E42" s="3">
         <v>42686</v>
@@ -1159,7 +1159,7 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E43" s="3">
         <v>42686</v>
@@ -1170,7 +1170,7 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E44" s="3">
         <v>42686</v>
@@ -1181,7 +1181,7 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E45" s="3">
         <v>42686</v>
@@ -1197,7 +1197,7 @@
         <v>46</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
@@ -1205,7 +1205,7 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
@@ -1213,7 +1213,7 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
@@ -1221,7 +1221,7 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
@@ -1229,7 +1229,7 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
finished 15 user stories, some changes in the Req Doc.
</commit_message>
<xml_diff>
--- a/Functional Requirements.xlsx
+++ b/Functional Requirements.xlsx
@@ -578,7 +578,7 @@
   <dimension ref="A1:G51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -859,7 +859,7 @@
         <v>15</v>
       </c>
       <c r="C16">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D16">
         <v>4</v>

</xml_diff>

<commit_message>
New requirements + User stories #31 - #35
</commit_message>
<xml_diff>
--- a/Functional Requirements.xlsx
+++ b/Functional Requirements.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="65">
   <si>
     <t>ID</t>
   </si>
@@ -187,6 +187,30 @@
   </si>
   <si>
     <t>Answer could be submited</t>
+  </si>
+  <si>
+    <t>Pupil will get a notification when he got a feedback</t>
+  </si>
+  <si>
+    <t>Pupils can be connected to a class</t>
+  </si>
+  <si>
+    <t>Teachers can be connected to a class</t>
+  </si>
+  <si>
+    <t>Pupils can be disconnected from a class</t>
+  </si>
+  <si>
+    <t>Teachers can be disconnected from a class</t>
+  </si>
+  <si>
+    <t>A class can be created</t>
+  </si>
+  <si>
+    <t>A class can be removed</t>
+  </si>
+  <si>
+    <t>Class details can be edited</t>
   </si>
 </sst>
 </file>
@@ -546,10 +570,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G51"/>
+  <dimension ref="A1:G61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E55" sqref="E55"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E62" sqref="E62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1555,6 +1579,176 @@
     <row r="51" spans="1:7">
       <c r="A51" s="1">
         <v>50</v>
+      </c>
+      <c r="B51" t="s">
+        <v>57</v>
+      </c>
+      <c r="C51" s="3">
+        <v>4</v>
+      </c>
+      <c r="D51" s="3">
+        <v>2</v>
+      </c>
+      <c r="E51" s="4">
+        <v>42686</v>
+      </c>
+      <c r="G51" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7">
+      <c r="A52" s="1">
+        <v>51</v>
+      </c>
+      <c r="B52" t="s">
+        <v>58</v>
+      </c>
+      <c r="C52" s="3">
+        <v>5</v>
+      </c>
+      <c r="D52" s="3">
+        <v>2</v>
+      </c>
+      <c r="E52" s="4">
+        <v>42686</v>
+      </c>
+      <c r="G52" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7">
+      <c r="A53" s="1">
+        <v>52</v>
+      </c>
+      <c r="B53" t="s">
+        <v>59</v>
+      </c>
+      <c r="C53" s="3">
+        <v>5</v>
+      </c>
+      <c r="D53" s="3">
+        <v>2</v>
+      </c>
+      <c r="E53" s="4">
+        <v>42686</v>
+      </c>
+      <c r="G53" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7">
+      <c r="A54" s="1">
+        <v>53</v>
+      </c>
+      <c r="B54" t="s">
+        <v>60</v>
+      </c>
+      <c r="C54" s="3">
+        <v>4</v>
+      </c>
+      <c r="D54" s="3">
+        <v>2</v>
+      </c>
+      <c r="E54" s="4">
+        <v>42686</v>
+      </c>
+      <c r="G54" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7">
+      <c r="A55" s="1">
+        <v>54</v>
+      </c>
+      <c r="B55" t="s">
+        <v>61</v>
+      </c>
+      <c r="C55" s="3">
+        <v>4</v>
+      </c>
+      <c r="D55" s="3">
+        <v>2</v>
+      </c>
+      <c r="E55" s="4">
+        <v>42686</v>
+      </c>
+      <c r="G55" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7">
+      <c r="A56" s="1">
+        <v>55</v>
+      </c>
+      <c r="B56" t="s">
+        <v>62</v>
+      </c>
+      <c r="C56" s="3">
+        <v>5</v>
+      </c>
+      <c r="D56" s="3">
+        <v>2</v>
+      </c>
+      <c r="E56" s="4">
+        <v>42686</v>
+      </c>
+      <c r="G56" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7">
+      <c r="A57" s="1">
+        <v>56</v>
+      </c>
+      <c r="B57" t="s">
+        <v>64</v>
+      </c>
+      <c r="C57" s="3">
+        <v>4</v>
+      </c>
+      <c r="D57" s="3">
+        <v>2</v>
+      </c>
+      <c r="E57" s="4">
+        <v>42686</v>
+      </c>
+      <c r="G57" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7">
+      <c r="A58" s="1">
+        <v>57</v>
+      </c>
+      <c r="B58" t="s">
+        <v>63</v>
+      </c>
+      <c r="C58" s="3">
+        <v>4</v>
+      </c>
+      <c r="D58" s="3">
+        <v>2</v>
+      </c>
+      <c r="E58" s="4">
+        <v>42686</v>
+      </c>
+      <c r="G58" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7">
+      <c r="A59" s="1">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7">
+      <c r="A60" s="1">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7">
+      <c r="A61" s="1">
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
two new req and priority and complexity for 15-30 reqs.
</commit_message>
<xml_diff>
--- a/Functional Requirements.xlsx
+++ b/Functional Requirements.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -11,12 +11,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="67">
   <si>
     <t>ID</t>
   </si>
@@ -211,6 +211,12 @@
   </si>
   <si>
     <t>Class details can be edited</t>
+  </si>
+  <si>
+    <t>pupils get notification on new texts that has been uploaded for them</t>
+  </si>
+  <si>
+    <t>pupils get notification on new question that has been uploaded for them</t>
   </si>
 </sst>
 </file>
@@ -254,7 +260,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -268,6 +274,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -286,7 +293,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="ערכת נושא Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -570,15 +577,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G61"/>
+  <dimension ref="A1:G65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F53" sqref="F53"/>
+    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="G67" sqref="G67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="2" max="2" width="52" customWidth="1"/>
+    <col min="2" max="2" width="56.5" customWidth="1"/>
     <col min="4" max="4" width="11.625" customWidth="1"/>
     <col min="5" max="5" width="19.375" customWidth="1"/>
     <col min="6" max="6" width="16.875" customWidth="1"/>
@@ -930,8 +937,12 @@
       <c r="B17" t="s">
         <v>16</v>
       </c>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
+      <c r="C17" s="3">
+        <v>2</v>
+      </c>
+      <c r="D17" s="3">
+        <v>3</v>
+      </c>
       <c r="E17" s="4">
         <v>42686</v>
       </c>
@@ -947,8 +958,12 @@
       <c r="B18" t="s">
         <v>17</v>
       </c>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
+      <c r="C18" s="3">
+        <v>5</v>
+      </c>
+      <c r="D18" s="3">
+        <v>4</v>
+      </c>
       <c r="E18" s="4">
         <v>42686</v>
       </c>
@@ -964,8 +979,12 @@
       <c r="B19" t="s">
         <v>18</v>
       </c>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
+      <c r="C19" s="3">
+        <v>3</v>
+      </c>
+      <c r="D19" s="3">
+        <v>2</v>
+      </c>
       <c r="E19" s="4">
         <v>42686</v>
       </c>
@@ -981,8 +1000,12 @@
       <c r="B20" t="s">
         <v>19</v>
       </c>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
+      <c r="C20" s="3">
+        <v>5</v>
+      </c>
+      <c r="D20" s="3">
+        <v>2</v>
+      </c>
       <c r="E20" s="4">
         <v>42686</v>
       </c>
@@ -998,8 +1021,12 @@
       <c r="B21" t="s">
         <v>20</v>
       </c>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
+      <c r="C21" s="3">
+        <v>5</v>
+      </c>
+      <c r="D21" s="3">
+        <v>2</v>
+      </c>
       <c r="E21" s="4">
         <v>42686</v>
       </c>
@@ -1015,8 +1042,12 @@
       <c r="B22" t="s">
         <v>23</v>
       </c>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
+      <c r="C22" s="3">
+        <v>5</v>
+      </c>
+      <c r="D22" s="3">
+        <v>2</v>
+      </c>
       <c r="E22" s="4">
         <v>42686</v>
       </c>
@@ -1032,8 +1063,12 @@
       <c r="B23" t="s">
         <v>21</v>
       </c>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
+      <c r="C23" s="3">
+        <v>5</v>
+      </c>
+      <c r="D23" s="3">
+        <v>3</v>
+      </c>
       <c r="E23" s="4">
         <v>42686</v>
       </c>
@@ -1049,8 +1084,12 @@
       <c r="B24" t="s">
         <v>22</v>
       </c>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
+      <c r="C24" s="3">
+        <v>5</v>
+      </c>
+      <c r="D24" s="3">
+        <v>2</v>
+      </c>
       <c r="E24" s="4">
         <v>42686</v>
       </c>
@@ -1066,8 +1105,12 @@
       <c r="B25" t="s">
         <v>24</v>
       </c>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
+      <c r="C25" s="3">
+        <v>5</v>
+      </c>
+      <c r="D25" s="3">
+        <v>2</v>
+      </c>
       <c r="E25" s="4">
         <v>42686</v>
       </c>
@@ -1083,8 +1126,12 @@
       <c r="B26" t="s">
         <v>25</v>
       </c>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
+      <c r="C26" s="3">
+        <v>5</v>
+      </c>
+      <c r="D26" s="3">
+        <v>2</v>
+      </c>
       <c r="E26" s="4">
         <v>42686</v>
       </c>
@@ -1100,8 +1147,12 @@
       <c r="B27" t="s">
         <v>26</v>
       </c>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
+      <c r="C27" s="3">
+        <v>5</v>
+      </c>
+      <c r="D27" s="3">
+        <v>2</v>
+      </c>
       <c r="E27" s="4">
         <v>42686</v>
       </c>
@@ -1117,8 +1168,12 @@
       <c r="B28" t="s">
         <v>27</v>
       </c>
-      <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
+      <c r="C28" s="3">
+        <v>5</v>
+      </c>
+      <c r="D28" s="3">
+        <v>2</v>
+      </c>
       <c r="E28" s="4">
         <v>42686</v>
       </c>
@@ -1134,8 +1189,12 @@
       <c r="B29" t="s">
         <v>28</v>
       </c>
-      <c r="C29" s="3"/>
-      <c r="D29" s="3"/>
+      <c r="C29" s="3">
+        <v>5</v>
+      </c>
+      <c r="D29" s="3">
+        <v>2</v>
+      </c>
       <c r="E29" s="4">
         <v>42686</v>
       </c>
@@ -1151,8 +1210,12 @@
       <c r="B30" t="s">
         <v>29</v>
       </c>
-      <c r="C30" s="3"/>
-      <c r="D30" s="3"/>
+      <c r="C30" s="3">
+        <v>5</v>
+      </c>
+      <c r="D30" s="3">
+        <v>2</v>
+      </c>
       <c r="E30" s="4">
         <v>42686</v>
       </c>
@@ -1168,8 +1231,12 @@
       <c r="B31" t="s">
         <v>30</v>
       </c>
-      <c r="C31" s="3"/>
-      <c r="D31" s="3"/>
+      <c r="C31" s="3">
+        <v>5</v>
+      </c>
+      <c r="D31" s="3">
+        <v>2</v>
+      </c>
       <c r="E31" s="4">
         <v>42686</v>
       </c>
@@ -1745,10 +1812,60 @@
       <c r="A60" s="1">
         <v>59</v>
       </c>
+      <c r="B60" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C60" s="3">
+        <v>3</v>
+      </c>
+      <c r="D60" s="3">
+        <v>3</v>
+      </c>
+      <c r="E60" s="4">
+        <v>42687</v>
+      </c>
+      <c r="G60" s="3" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="61" spans="1:7">
       <c r="A61" s="1">
         <v>60</v>
+      </c>
+      <c r="B61" t="s">
+        <v>66</v>
+      </c>
+      <c r="C61" s="3">
+        <v>3</v>
+      </c>
+      <c r="D61" s="3">
+        <v>3</v>
+      </c>
+      <c r="E61" s="4">
+        <v>42687</v>
+      </c>
+      <c r="G61" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7">
+      <c r="A62" s="1">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7">
+      <c r="A63" s="1">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7">
+      <c r="A64" s="1">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1">
+      <c r="A65" s="1">
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
functional req + user stories for #45-#50.
</commit_message>
<xml_diff>
--- a/Functional Requirements.xlsx
+++ b/Functional Requirements.xlsx
@@ -579,8 +579,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="G67" sqref="G67"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="B52" sqref="B52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1807,13 +1807,28 @@
       <c r="A59" s="1">
         <v>58</v>
       </c>
+      <c r="B59" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C59" s="3">
+        <v>3</v>
+      </c>
+      <c r="D59" s="3">
+        <v>3</v>
+      </c>
+      <c r="E59" s="4">
+        <v>42687</v>
+      </c>
+      <c r="G59" s="3" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="60" spans="1:7">
       <c r="A60" s="1">
         <v>59</v>
       </c>
-      <c r="B60" s="5" t="s">
-        <v>65</v>
+      <c r="B60" t="s">
+        <v>66</v>
       </c>
       <c r="C60" s="3">
         <v>3</v>
@@ -1831,21 +1846,6 @@
     <row r="61" spans="1:7">
       <c r="A61" s="1">
         <v>60</v>
-      </c>
-      <c r="B61" t="s">
-        <v>66</v>
-      </c>
-      <c r="C61" s="3">
-        <v>3</v>
-      </c>
-      <c r="D61" s="3">
-        <v>3</v>
-      </c>
-      <c r="E61" s="4">
-        <v>42687</v>
-      </c>
-      <c r="G61" s="3" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="62" spans="1:7">

</xml_diff>

<commit_message>
finish requirements and user stories #51-59..
</commit_message>
<xml_diff>
--- a/Functional Requirements.xlsx
+++ b/Functional Requirements.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="70">
   <si>
     <t>ID</t>
   </si>
@@ -213,10 +213,19 @@
     <t>Class details can be edited</t>
   </si>
   <si>
-    <t>pupils get notification on new texts that has been uploaded for them</t>
-  </si>
-  <si>
-    <t>pupils get notification on new question that has been uploaded for them</t>
+    <t>"       "          "        "</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"       "          "        " </t>
+  </si>
+  <si>
+    <t>permission for teachers as well?</t>
+  </si>
+  <si>
+    <t>pupils get notification on new texts that have been uploaded for them</t>
+  </si>
+  <si>
+    <t>pupils get notification on new question that have been uploaded for them</t>
   </si>
 </sst>
 </file>
@@ -577,10 +586,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G65"/>
+  <dimension ref="A1:H65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="B52" sqref="B52"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="B60" sqref="B60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -590,6 +599,7 @@
     <col min="5" max="5" width="19.375" customWidth="1"/>
     <col min="6" max="6" width="16.875" customWidth="1"/>
     <col min="7" max="7" width="16.375" customWidth="1"/>
+    <col min="8" max="8" width="19.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15">
@@ -1602,7 +1612,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="49" spans="1:7">
+    <row r="49" spans="1:8">
       <c r="A49" s="1">
         <v>48</v>
       </c>
@@ -1623,7 +1633,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="50" spans="1:7">
+    <row r="50" spans="1:8">
       <c r="A50" s="1">
         <v>49</v>
       </c>
@@ -1643,7 +1653,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="51" spans="1:7">
+    <row r="51" spans="1:8">
       <c r="A51" s="1">
         <v>50</v>
       </c>
@@ -1663,7 +1673,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="52" spans="1:7">
+    <row r="52" spans="1:8">
       <c r="A52" s="1">
         <v>51</v>
       </c>
@@ -1683,7 +1693,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="53" spans="1:7">
+    <row r="53" spans="1:8">
       <c r="A53" s="1">
         <v>52</v>
       </c>
@@ -1703,7 +1713,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="54" spans="1:7">
+    <row r="54" spans="1:8">
       <c r="A54" s="1">
         <v>53</v>
       </c>
@@ -1723,7 +1733,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="55" spans="1:7">
+    <row r="55" spans="1:8">
       <c r="A55" s="1">
         <v>54</v>
       </c>
@@ -1743,7 +1753,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="56" spans="1:7">
+    <row r="56" spans="1:8">
       <c r="A56" s="1">
         <v>55</v>
       </c>
@@ -1762,8 +1772,11 @@
       <c r="G56" s="3" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="57" spans="1:7">
+      <c r="H56" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8">
       <c r="A57" s="1">
         <v>56</v>
       </c>
@@ -1782,8 +1795,11 @@
       <c r="G57" s="3" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="58" spans="1:7">
+      <c r="H57" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8">
       <c r="A58" s="1">
         <v>57</v>
       </c>
@@ -1802,13 +1818,16 @@
       <c r="G58" s="3" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="59" spans="1:7">
+      <c r="H58" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8">
       <c r="A59" s="1">
         <v>58</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="C59" s="3">
         <v>3</v>
@@ -1823,12 +1842,12 @@
         <v>55</v>
       </c>
     </row>
-    <row r="60" spans="1:7">
+    <row r="60" spans="1:8">
       <c r="A60" s="1">
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="C60" s="3">
         <v>3</v>
@@ -1843,22 +1862,22 @@
         <v>55</v>
       </c>
     </row>
-    <row r="61" spans="1:7">
+    <row r="61" spans="1:8">
       <c r="A61" s="1">
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:7">
+    <row r="62" spans="1:8">
       <c r="A62" s="1">
         <v>61</v>
       </c>
     </row>
-    <row r="63" spans="1:7">
+    <row r="63" spans="1:8">
       <c r="A63" s="1">
         <v>62</v>
       </c>
     </row>
-    <row r="64" spans="1:7">
+    <row r="64" spans="1:8">
       <c r="A64" s="1">
         <v>63</v>
       </c>

</xml_diff>

<commit_message>
User stories #36 - #44, #51 - #57 + new requirments
</commit_message>
<xml_diff>
--- a/Functional Requirements.xlsx
+++ b/Functional Requirements.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -11,12 +11,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="73">
   <si>
     <t>ID</t>
   </si>
@@ -213,19 +213,28 @@
     <t>Class details can be edited</t>
   </si>
   <si>
-    <t>"       "          "        "</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"       "          "        " </t>
-  </si>
-  <si>
-    <t>permission for teachers as well?</t>
-  </si>
-  <si>
-    <t>pupils get notification on new texts that have been uploaded for them</t>
-  </si>
-  <si>
-    <t>pupils get notification on new question that have been uploaded for them</t>
+    <t>pupils get notification for new uploaded assignment</t>
+  </si>
+  <si>
+    <t>The list of all of the classes can be viewed</t>
+  </si>
+  <si>
+    <t>The list of all of the pupils in a specific class can be viewed</t>
+  </si>
+  <si>
+    <t>The list of all of the teachers in a specific class can be viewed</t>
+  </si>
+  <si>
+    <t>Teacher's details can be viewed be clicking on him</t>
+  </si>
+  <si>
+    <t>Pupil's details can be viewed by clicking on him</t>
+  </si>
+  <si>
+    <t>The list of all of the teachers can be viewed</t>
+  </si>
+  <si>
+    <t>The list of all of the pupils can be viewed</t>
   </si>
 </sst>
 </file>
@@ -302,7 +311,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="ערכת נושא Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -586,10 +595,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H65"/>
+  <dimension ref="A1:G71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="B60" sqref="B60"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="C69" sqref="C69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1536,7 +1545,7 @@
         <v>43</v>
       </c>
       <c r="C45" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D45" s="3">
         <v>1</v>
@@ -1612,7 +1621,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="49" spans="1:8">
+    <row r="49" spans="1:7">
       <c r="A49" s="1">
         <v>48</v>
       </c>
@@ -1633,7 +1642,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="50" spans="1:8">
+    <row r="50" spans="1:7">
       <c r="A50" s="1">
         <v>49</v>
       </c>
@@ -1653,7 +1662,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="51" spans="1:8">
+    <row r="51" spans="1:7">
       <c r="A51" s="1">
         <v>50</v>
       </c>
@@ -1673,7 +1682,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="52" spans="1:8">
+    <row r="52" spans="1:7">
       <c r="A52" s="1">
         <v>51</v>
       </c>
@@ -1693,7 +1702,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="53" spans="1:8">
+    <row r="53" spans="1:7">
       <c r="A53" s="1">
         <v>52</v>
       </c>
@@ -1713,7 +1722,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="54" spans="1:8">
+    <row r="54" spans="1:7">
       <c r="A54" s="1">
         <v>53</v>
       </c>
@@ -1733,7 +1742,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="55" spans="1:8">
+    <row r="55" spans="1:7">
       <c r="A55" s="1">
         <v>54</v>
       </c>
@@ -1753,7 +1762,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="56" spans="1:8">
+    <row r="56" spans="1:7">
       <c r="A56" s="1">
         <v>55</v>
       </c>
@@ -1772,11 +1781,8 @@
       <c r="G56" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="H56" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8">
+    </row>
+    <row r="57" spans="1:7">
       <c r="A57" s="1">
         <v>56</v>
       </c>
@@ -1795,11 +1801,8 @@
       <c r="G57" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="H57" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8">
+    </row>
+    <row r="58" spans="1:7">
       <c r="A58" s="1">
         <v>57</v>
       </c>
@@ -1818,16 +1821,13 @@
       <c r="G58" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="H58" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8">
+    </row>
+    <row r="59" spans="1:7">
       <c r="A59" s="1">
         <v>58</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C59" s="3">
         <v>3</v>
@@ -1842,49 +1842,169 @@
         <v>55</v>
       </c>
     </row>
-    <row r="60" spans="1:8">
+    <row r="60" spans="1:7">
       <c r="A60" s="1">
         <v>59</v>
       </c>
-      <c r="B60" t="s">
-        <v>69</v>
+      <c r="B60" s="5" t="s">
+        <v>66</v>
       </c>
       <c r="C60" s="3">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D60" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E60" s="4">
-        <v>42687</v>
+        <v>42690</v>
       </c>
       <c r="G60" s="3" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="61" spans="1:8">
+    <row r="61" spans="1:7">
       <c r="A61" s="1">
         <v>60</v>
       </c>
-    </row>
-    <row r="62" spans="1:8">
+      <c r="B61" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C61" s="3">
+        <v>5</v>
+      </c>
+      <c r="D61" s="3">
+        <v>2</v>
+      </c>
+      <c r="E61" s="4">
+        <v>42690</v>
+      </c>
+      <c r="G61" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7">
       <c r="A62" s="1">
         <v>61</v>
       </c>
-    </row>
-    <row r="63" spans="1:8">
+      <c r="B62" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C62" s="3">
+        <v>5</v>
+      </c>
+      <c r="D62" s="3">
+        <v>2</v>
+      </c>
+      <c r="E62" s="4">
+        <v>42690</v>
+      </c>
+      <c r="G62" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7">
       <c r="A63" s="1">
         <v>62</v>
       </c>
-    </row>
-    <row r="64" spans="1:8">
+      <c r="B63" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C63" s="3">
+        <v>5</v>
+      </c>
+      <c r="D63" s="3">
+        <v>2</v>
+      </c>
+      <c r="E63" s="4">
+        <v>42690</v>
+      </c>
+      <c r="G63" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7">
       <c r="A64" s="1">
         <v>63</v>
       </c>
-    </row>
-    <row r="65" spans="1:1">
+      <c r="B64" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C64" s="3">
+        <v>5</v>
+      </c>
+      <c r="D64" s="3">
+        <v>2</v>
+      </c>
+      <c r="E64" s="4">
+        <v>42690</v>
+      </c>
+      <c r="G64" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7">
       <c r="A65" s="1">
         <v>64</v>
+      </c>
+      <c r="B65" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C65" s="3">
+        <v>5</v>
+      </c>
+      <c r="D65" s="3">
+        <v>2</v>
+      </c>
+      <c r="E65" s="4">
+        <v>42690</v>
+      </c>
+      <c r="G65" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7">
+      <c r="A66" s="1">
+        <v>65</v>
+      </c>
+      <c r="B66" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C66" s="3">
+        <v>5</v>
+      </c>
+      <c r="D66" s="3">
+        <v>2</v>
+      </c>
+      <c r="E66" s="4">
+        <v>42690</v>
+      </c>
+      <c r="G66" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7">
+      <c r="A67" s="1">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7">
+      <c r="A68" s="1">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7">
+      <c r="A69" s="1">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7">
+      <c r="A70" s="1">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7">
+      <c r="A71" s="1">
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed requirements according to Arnon's notes
</commit_message>
<xml_diff>
--- a/Functional Requirements.xlsx
+++ b/Functional Requirements.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17426"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -39,9 +39,6 @@
     <t>Status</t>
   </si>
   <si>
-    <t>Ability to answer questions related to a text</t>
-  </si>
-  <si>
     <t>Feedback for number of words in an answer</t>
   </si>
   <si>
@@ -235,13 +232,16 @@
   </si>
   <si>
     <t>The list of all of the pupils can be viewed</t>
+  </si>
+  <si>
+    <t>Ability to answer questions related to a text after reading it</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -353,7 +353,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -385,9 +385,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -419,6 +437,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -594,14 +630,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="C69" sqref="C69"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" activeCellId="1" sqref="B8 B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="56.5" customWidth="1"/>
     <col min="4" max="4" width="11.625" customWidth="1"/>
@@ -611,7 +647,7 @@
     <col min="8" max="8" width="19.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15">
+    <row r="1" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -634,12 +670,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C2" s="3">
         <v>5</v>
@@ -652,15 +688,15 @@
       </c>
       <c r="F2" s="3"/>
       <c r="G2" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C3" s="3">
         <v>4</v>
@@ -673,15 +709,15 @@
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C4" s="3">
         <v>1</v>
@@ -694,15 +730,15 @@
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C5" s="3">
         <v>5</v>
@@ -715,15 +751,15 @@
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>72</v>
       </c>
       <c r="C6" s="3">
         <v>5</v>
@@ -736,15 +772,15 @@
       </c>
       <c r="F6" s="3"/>
       <c r="G6" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C7" s="3">
         <v>5</v>
@@ -757,15 +793,15 @@
       </c>
       <c r="F7" s="3"/>
       <c r="G7" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C8" s="3">
         <v>5</v>
@@ -778,15 +814,15 @@
       </c>
       <c r="F8" s="3"/>
       <c r="G8" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C9" s="3">
         <v>5</v>
@@ -799,15 +835,15 @@
       </c>
       <c r="F9" s="3"/>
       <c r="G9" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C10" s="3">
         <v>5</v>
@@ -820,15 +856,15 @@
       </c>
       <c r="F10" s="3"/>
       <c r="G10" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C11" s="3">
         <v>5</v>
@@ -841,15 +877,15 @@
       </c>
       <c r="F11" s="3"/>
       <c r="G11" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C12" s="3">
         <v>4</v>
@@ -862,15 +898,15 @@
       </c>
       <c r="F12" s="3"/>
       <c r="G12" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C13" s="3">
         <v>4</v>
@@ -883,15 +919,15 @@
       </c>
       <c r="F13" s="3"/>
       <c r="G13" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C14" s="3">
         <v>3</v>
@@ -904,15 +940,15 @@
       </c>
       <c r="F14" s="3"/>
       <c r="G14" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C15" s="3">
         <v>3</v>
@@ -925,15 +961,15 @@
       </c>
       <c r="F15" s="3"/>
       <c r="G15" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C16" s="3">
         <v>3</v>
@@ -946,15 +982,15 @@
       </c>
       <c r="F16" s="3"/>
       <c r="G16" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C17" s="3">
         <v>2</v>
@@ -967,15 +1003,15 @@
       </c>
       <c r="F17" s="3"/>
       <c r="G17" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C18" s="3">
         <v>5</v>
@@ -988,15 +1024,15 @@
       </c>
       <c r="F18" s="3"/>
       <c r="G18" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C19" s="3">
         <v>3</v>
@@ -1009,15 +1045,15 @@
       </c>
       <c r="F19" s="3"/>
       <c r="G19" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C20" s="3">
         <v>5</v>
@@ -1030,15 +1066,15 @@
       </c>
       <c r="F20" s="3"/>
       <c r="G20" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C21" s="3">
         <v>5</v>
@@ -1051,15 +1087,15 @@
       </c>
       <c r="F21" s="3"/>
       <c r="G21" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C22" s="3">
         <v>5</v>
@@ -1072,15 +1108,15 @@
       </c>
       <c r="F22" s="3"/>
       <c r="G22" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C23" s="3">
         <v>5</v>
@@ -1093,15 +1129,15 @@
       </c>
       <c r="F23" s="3"/>
       <c r="G23" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C24" s="3">
         <v>5</v>
@@ -1114,15 +1150,15 @@
       </c>
       <c r="F24" s="3"/>
       <c r="G24" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C25" s="3">
         <v>5</v>
@@ -1135,15 +1171,15 @@
       </c>
       <c r="F25" s="3"/>
       <c r="G25" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C26" s="3">
         <v>5</v>
@@ -1156,15 +1192,15 @@
       </c>
       <c r="F26" s="3"/>
       <c r="G26" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C27" s="3">
         <v>5</v>
@@ -1177,15 +1213,15 @@
       </c>
       <c r="F27" s="3"/>
       <c r="G27" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C28" s="3">
         <v>5</v>
@@ -1198,15 +1234,15 @@
       </c>
       <c r="F28" s="3"/>
       <c r="G28" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C29" s="3">
         <v>5</v>
@@ -1219,15 +1255,15 @@
       </c>
       <c r="F29" s="3"/>
       <c r="G29" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C30" s="3">
         <v>5</v>
@@ -1240,15 +1276,15 @@
       </c>
       <c r="F30" s="3"/>
       <c r="G30" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C31" s="3">
         <v>5</v>
@@ -1261,15 +1297,15 @@
       </c>
       <c r="F31" s="3"/>
       <c r="G31" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C32" s="3">
         <v>5</v>
@@ -1282,15 +1318,15 @@
       </c>
       <c r="F32" s="3"/>
       <c r="G32" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C33" s="3">
         <v>4</v>
@@ -1303,15 +1339,15 @@
       </c>
       <c r="F33" s="3"/>
       <c r="G33" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C34" s="3">
         <v>4</v>
@@ -1324,15 +1360,15 @@
       </c>
       <c r="F34" s="3"/>
       <c r="G34" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C35" s="3">
         <v>4</v>
@@ -1345,15 +1381,15 @@
       </c>
       <c r="F35" s="3"/>
       <c r="G35" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C36" s="3">
         <v>5</v>
@@ -1366,15 +1402,15 @@
       </c>
       <c r="F36" s="3"/>
       <c r="G36" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C37" s="3">
         <v>2</v>
@@ -1387,15 +1423,15 @@
       </c>
       <c r="F37" s="3"/>
       <c r="G37" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C38" s="3">
         <v>5</v>
@@ -1408,15 +1444,15 @@
       </c>
       <c r="F38" s="3"/>
       <c r="G38" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C39" s="3">
         <v>4</v>
@@ -1429,15 +1465,15 @@
       </c>
       <c r="F39" s="3"/>
       <c r="G39" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C40" s="3">
         <v>4</v>
@@ -1450,15 +1486,15 @@
       </c>
       <c r="F40" s="3"/>
       <c r="G40" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C41" s="3">
         <v>5</v>
@@ -1471,15 +1507,15 @@
       </c>
       <c r="F41" s="3"/>
       <c r="G41" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C42" s="3">
         <v>4</v>
@@ -1492,15 +1528,15 @@
       </c>
       <c r="F42" s="3"/>
       <c r="G42" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C43" s="3">
         <v>4</v>
@@ -1513,15 +1549,15 @@
       </c>
       <c r="F43" s="3"/>
       <c r="G43" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C44" s="3">
         <v>3</v>
@@ -1534,15 +1570,15 @@
       </c>
       <c r="F44" s="3"/>
       <c r="G44" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C45" s="3">
         <v>1</v>
@@ -1555,15 +1591,15 @@
       </c>
       <c r="F45" s="3"/>
       <c r="G45" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C46" s="3">
         <v>5</v>
@@ -1576,15 +1612,15 @@
       </c>
       <c r="F46" s="3"/>
       <c r="G46" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C47" s="3">
         <v>4</v>
@@ -1597,15 +1633,15 @@
       </c>
       <c r="F47" s="3"/>
       <c r="G47" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C48" s="3">
         <v>5</v>
@@ -1618,15 +1654,15 @@
       </c>
       <c r="F48" s="3"/>
       <c r="G48" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C49" s="3">
         <v>4</v>
@@ -1639,15 +1675,15 @@
       </c>
       <c r="F49" s="3"/>
       <c r="G49" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C50" s="3">
         <v>5</v>
@@ -1659,15 +1695,15 @@
         <v>42687</v>
       </c>
       <c r="G50" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C51" s="3">
         <v>4</v>
@@ -1679,15 +1715,15 @@
         <v>42687</v>
       </c>
       <c r="G51" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C52" s="3">
         <v>5</v>
@@ -1699,15 +1735,15 @@
         <v>42687</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C53" s="3">
         <v>5</v>
@@ -1719,15 +1755,15 @@
         <v>42687</v>
       </c>
       <c r="G53" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C54" s="3">
         <v>4</v>
@@ -1739,15 +1775,15 @@
         <v>42687</v>
       </c>
       <c r="G54" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C55" s="3">
         <v>4</v>
@@ -1759,15 +1795,15 @@
         <v>42687</v>
       </c>
       <c r="G55" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C56" s="3">
         <v>5</v>
@@ -1779,15 +1815,15 @@
         <v>42687</v>
       </c>
       <c r="G56" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C57" s="3">
         <v>4</v>
@@ -1799,15 +1835,15 @@
         <v>42687</v>
       </c>
       <c r="G57" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C58" s="3">
         <v>4</v>
@@ -1819,15 +1855,15 @@
         <v>42687</v>
       </c>
       <c r="G58" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
         <v>58</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C59" s="3">
         <v>3</v>
@@ -1839,15 +1875,15 @@
         <v>42687</v>
       </c>
       <c r="G59" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
         <v>59</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C60" s="3">
         <v>5</v>
@@ -1859,15 +1895,15 @@
         <v>42690</v>
       </c>
       <c r="G60" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
         <v>60</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C61" s="3">
         <v>5</v>
@@ -1879,15 +1915,15 @@
         <v>42690</v>
       </c>
       <c r="G61" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
         <v>61</v>
       </c>
       <c r="B62" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C62" s="3">
         <v>5</v>
@@ -1899,15 +1935,15 @@
         <v>42690</v>
       </c>
       <c r="G62" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
         <v>62</v>
       </c>
       <c r="B63" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C63" s="3">
         <v>5</v>
@@ -1919,15 +1955,15 @@
         <v>42690</v>
       </c>
       <c r="G63" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
         <v>63</v>
       </c>
       <c r="B64" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C64" s="3">
         <v>5</v>
@@ -1939,15 +1975,15 @@
         <v>42690</v>
       </c>
       <c r="G64" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
         <v>64</v>
       </c>
       <c r="B65" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C65" s="3">
         <v>5</v>
@@ -1959,15 +1995,15 @@
         <v>42690</v>
       </c>
       <c r="G65" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
         <v>65</v>
       </c>
       <c r="B66" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C66" s="3">
         <v>5</v>
@@ -1979,30 +2015,30 @@
         <v>42690</v>
       </c>
       <c r="G66" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
         <v>66</v>
       </c>
     </row>
-    <row r="68" spans="1:7">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
         <v>67</v>
       </c>
     </row>
-    <row r="69" spans="1:7">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
         <v>68</v>
       </c>
     </row>
-    <row r="70" spans="1:7">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
         <v>69</v>
       </c>
     </row>
-    <row r="71" spans="1:7">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A71" s="1">
         <v>70</v>
       </c>
@@ -2014,26 +2050,26 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Done with Req Doc, fixing user stories.
</commit_message>
<xml_diff>
--- a/Functional Requirements.xlsx
+++ b/Functional Requirements.xlsx
@@ -66,9 +66,6 @@
     <t>Ability to compare between scores of other pupils</t>
   </si>
   <si>
-    <t>Check button for feedbacking all the answer's parameters</t>
-  </si>
-  <si>
     <t>Marking and correcting sequence of repeated words</t>
   </si>
   <si>
@@ -235,6 +232,9 @@
   </si>
   <si>
     <t>Ability to answer questions related to a text after reading it</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Check" button - upon clicking the pupil recieves feedback for answer  </t>
   </si>
 </sst>
 </file>
@@ -634,7 +634,7 @@
   <dimension ref="A1:G71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" activeCellId="1" sqref="B8 B8"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -675,7 +675,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C2" s="3">
         <v>5</v>
@@ -688,7 +688,7 @@
       </c>
       <c r="F2" s="3"/>
       <c r="G2" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -696,7 +696,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C3" s="3">
         <v>4</v>
@@ -709,7 +709,7 @@
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -717,7 +717,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C4" s="3">
         <v>1</v>
@@ -730,7 +730,7 @@
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -738,7 +738,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C5" s="3">
         <v>5</v>
@@ -751,7 +751,7 @@
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -759,7 +759,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C6" s="3">
         <v>5</v>
@@ -772,7 +772,7 @@
       </c>
       <c r="F6" s="3"/>
       <c r="G6" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -793,7 +793,7 @@
       </c>
       <c r="F7" s="3"/>
       <c r="G7" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -814,7 +814,7 @@
       </c>
       <c r="F8" s="3"/>
       <c r="G8" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -835,7 +835,7 @@
       </c>
       <c r="F9" s="3"/>
       <c r="G9" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
@@ -856,7 +856,7 @@
       </c>
       <c r="F10" s="3"/>
       <c r="G10" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -877,7 +877,7 @@
       </c>
       <c r="F11" s="3"/>
       <c r="G11" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
@@ -885,7 +885,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C12" s="3">
         <v>4</v>
@@ -898,7 +898,7 @@
       </c>
       <c r="F12" s="3"/>
       <c r="G12" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
@@ -906,7 +906,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C13" s="3">
         <v>4</v>
@@ -919,7 +919,7 @@
       </c>
       <c r="F13" s="3"/>
       <c r="G13" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
@@ -940,7 +940,7 @@
       </c>
       <c r="F14" s="3"/>
       <c r="G14" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
@@ -961,7 +961,7 @@
       </c>
       <c r="F15" s="3"/>
       <c r="G15" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
@@ -982,7 +982,7 @@
       </c>
       <c r="F16" s="3"/>
       <c r="G16" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
@@ -1003,7 +1003,7 @@
       </c>
       <c r="F17" s="3"/>
       <c r="G17" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
@@ -1011,7 +1011,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>16</v>
+        <v>72</v>
       </c>
       <c r="C18" s="3">
         <v>5</v>
@@ -1024,7 +1024,7 @@
       </c>
       <c r="F18" s="3"/>
       <c r="G18" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
@@ -1032,7 +1032,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C19" s="3">
         <v>3</v>
@@ -1045,7 +1045,7 @@
       </c>
       <c r="F19" s="3"/>
       <c r="G19" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
@@ -1053,7 +1053,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C20" s="3">
         <v>5</v>
@@ -1066,7 +1066,7 @@
       </c>
       <c r="F20" s="3"/>
       <c r="G20" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
@@ -1074,7 +1074,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C21" s="3">
         <v>5</v>
@@ -1087,7 +1087,7 @@
       </c>
       <c r="F21" s="3"/>
       <c r="G21" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
@@ -1095,7 +1095,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C22" s="3">
         <v>5</v>
@@ -1108,7 +1108,7 @@
       </c>
       <c r="F22" s="3"/>
       <c r="G22" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
@@ -1116,7 +1116,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C23" s="3">
         <v>5</v>
@@ -1129,7 +1129,7 @@
       </c>
       <c r="F23" s="3"/>
       <c r="G23" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
@@ -1137,7 +1137,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C24" s="3">
         <v>5</v>
@@ -1150,7 +1150,7 @@
       </c>
       <c r="F24" s="3"/>
       <c r="G24" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
@@ -1158,7 +1158,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C25" s="3">
         <v>5</v>
@@ -1171,7 +1171,7 @@
       </c>
       <c r="F25" s="3"/>
       <c r="G25" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
@@ -1179,7 +1179,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C26" s="3">
         <v>5</v>
@@ -1192,7 +1192,7 @@
       </c>
       <c r="F26" s="3"/>
       <c r="G26" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
@@ -1200,7 +1200,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C27" s="3">
         <v>5</v>
@@ -1213,7 +1213,7 @@
       </c>
       <c r="F27" s="3"/>
       <c r="G27" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
@@ -1221,7 +1221,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C28" s="3">
         <v>5</v>
@@ -1234,7 +1234,7 @@
       </c>
       <c r="F28" s="3"/>
       <c r="G28" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
@@ -1242,7 +1242,7 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C29" s="3">
         <v>5</v>
@@ -1255,7 +1255,7 @@
       </c>
       <c r="F29" s="3"/>
       <c r="G29" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
@@ -1263,7 +1263,7 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C30" s="3">
         <v>5</v>
@@ -1276,7 +1276,7 @@
       </c>
       <c r="F30" s="3"/>
       <c r="G30" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
@@ -1284,7 +1284,7 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C31" s="3">
         <v>5</v>
@@ -1297,7 +1297,7 @@
       </c>
       <c r="F31" s="3"/>
       <c r="G31" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
@@ -1305,7 +1305,7 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C32" s="3">
         <v>5</v>
@@ -1318,7 +1318,7 @@
       </c>
       <c r="F32" s="3"/>
       <c r="G32" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
@@ -1326,7 +1326,7 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C33" s="3">
         <v>4</v>
@@ -1339,7 +1339,7 @@
       </c>
       <c r="F33" s="3"/>
       <c r="G33" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
@@ -1347,7 +1347,7 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C34" s="3">
         <v>4</v>
@@ -1360,7 +1360,7 @@
       </c>
       <c r="F34" s="3"/>
       <c r="G34" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
@@ -1368,7 +1368,7 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C35" s="3">
         <v>4</v>
@@ -1381,7 +1381,7 @@
       </c>
       <c r="F35" s="3"/>
       <c r="G35" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
@@ -1389,7 +1389,7 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C36" s="3">
         <v>5</v>
@@ -1402,7 +1402,7 @@
       </c>
       <c r="F36" s="3"/>
       <c r="G36" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
@@ -1410,7 +1410,7 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C37" s="3">
         <v>2</v>
@@ -1423,7 +1423,7 @@
       </c>
       <c r="F37" s="3"/>
       <c r="G37" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
@@ -1431,7 +1431,7 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C38" s="3">
         <v>5</v>
@@ -1444,7 +1444,7 @@
       </c>
       <c r="F38" s="3"/>
       <c r="G38" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
@@ -1452,7 +1452,7 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C39" s="3">
         <v>4</v>
@@ -1465,7 +1465,7 @@
       </c>
       <c r="F39" s="3"/>
       <c r="G39" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
@@ -1473,7 +1473,7 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C40" s="3">
         <v>4</v>
@@ -1486,7 +1486,7 @@
       </c>
       <c r="F40" s="3"/>
       <c r="G40" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
@@ -1494,7 +1494,7 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C41" s="3">
         <v>5</v>
@@ -1507,7 +1507,7 @@
       </c>
       <c r="F41" s="3"/>
       <c r="G41" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
@@ -1515,7 +1515,7 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C42" s="3">
         <v>4</v>
@@ -1528,7 +1528,7 @@
       </c>
       <c r="F42" s="3"/>
       <c r="G42" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
@@ -1536,7 +1536,7 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C43" s="3">
         <v>4</v>
@@ -1549,7 +1549,7 @@
       </c>
       <c r="F43" s="3"/>
       <c r="G43" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
@@ -1557,7 +1557,7 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C44" s="3">
         <v>3</v>
@@ -1570,7 +1570,7 @@
       </c>
       <c r="F44" s="3"/>
       <c r="G44" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
@@ -1578,7 +1578,7 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C45" s="3">
         <v>1</v>
@@ -1591,7 +1591,7 @@
       </c>
       <c r="F45" s="3"/>
       <c r="G45" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
@@ -1599,7 +1599,7 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C46" s="3">
         <v>5</v>
@@ -1612,7 +1612,7 @@
       </c>
       <c r="F46" s="3"/>
       <c r="G46" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
@@ -1620,7 +1620,7 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C47" s="3">
         <v>4</v>
@@ -1633,7 +1633,7 @@
       </c>
       <c r="F47" s="3"/>
       <c r="G47" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
@@ -1641,7 +1641,7 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C48" s="3">
         <v>5</v>
@@ -1654,7 +1654,7 @@
       </c>
       <c r="F48" s="3"/>
       <c r="G48" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.2">
@@ -1662,7 +1662,7 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C49" s="3">
         <v>4</v>
@@ -1675,7 +1675,7 @@
       </c>
       <c r="F49" s="3"/>
       <c r="G49" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.2">
@@ -1683,7 +1683,7 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C50" s="3">
         <v>5</v>
@@ -1695,7 +1695,7 @@
         <v>42687</v>
       </c>
       <c r="G50" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
@@ -1703,7 +1703,7 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C51" s="3">
         <v>4</v>
@@ -1715,7 +1715,7 @@
         <v>42687</v>
       </c>
       <c r="G51" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.2">
@@ -1723,7 +1723,7 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C52" s="3">
         <v>5</v>
@@ -1735,7 +1735,7 @@
         <v>42687</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.2">
@@ -1743,7 +1743,7 @@
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C53" s="3">
         <v>5</v>
@@ -1755,7 +1755,7 @@
         <v>42687</v>
       </c>
       <c r="G53" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.2">
@@ -1763,7 +1763,7 @@
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C54" s="3">
         <v>4</v>
@@ -1775,7 +1775,7 @@
         <v>42687</v>
       </c>
       <c r="G54" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.2">
@@ -1783,7 +1783,7 @@
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C55" s="3">
         <v>4</v>
@@ -1795,7 +1795,7 @@
         <v>42687</v>
       </c>
       <c r="G55" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.2">
@@ -1803,7 +1803,7 @@
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C56" s="3">
         <v>5</v>
@@ -1815,7 +1815,7 @@
         <v>42687</v>
       </c>
       <c r="G56" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.2">
@@ -1823,7 +1823,7 @@
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C57" s="3">
         <v>4</v>
@@ -1835,7 +1835,7 @@
         <v>42687</v>
       </c>
       <c r="G57" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.2">
@@ -1843,7 +1843,7 @@
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C58" s="3">
         <v>4</v>
@@ -1855,7 +1855,7 @@
         <v>42687</v>
       </c>
       <c r="G58" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.2">
@@ -1863,7 +1863,7 @@
         <v>58</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C59" s="3">
         <v>3</v>
@@ -1875,7 +1875,7 @@
         <v>42687</v>
       </c>
       <c r="G59" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.2">
@@ -1883,7 +1883,7 @@
         <v>59</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C60" s="3">
         <v>5</v>
@@ -1895,7 +1895,7 @@
         <v>42690</v>
       </c>
       <c r="G60" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.2">
@@ -1903,7 +1903,7 @@
         <v>60</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C61" s="3">
         <v>5</v>
@@ -1915,7 +1915,7 @@
         <v>42690</v>
       </c>
       <c r="G61" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.2">
@@ -1923,7 +1923,7 @@
         <v>61</v>
       </c>
       <c r="B62" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C62" s="3">
         <v>5</v>
@@ -1935,7 +1935,7 @@
         <v>42690</v>
       </c>
       <c r="G62" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.2">
@@ -1943,7 +1943,7 @@
         <v>62</v>
       </c>
       <c r="B63" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C63" s="3">
         <v>5</v>
@@ -1955,7 +1955,7 @@
         <v>42690</v>
       </c>
       <c r="G63" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.2">
@@ -1963,7 +1963,7 @@
         <v>63</v>
       </c>
       <c r="B64" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C64" s="3">
         <v>5</v>
@@ -1975,7 +1975,7 @@
         <v>42690</v>
       </c>
       <c r="G64" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.2">
@@ -1983,7 +1983,7 @@
         <v>64</v>
       </c>
       <c r="B65" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C65" s="3">
         <v>5</v>
@@ -1995,7 +1995,7 @@
         <v>42690</v>
       </c>
       <c r="G65" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.2">
@@ -2003,7 +2003,7 @@
         <v>65</v>
       </c>
       <c r="B66" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C66" s="3">
         <v>5</v>
@@ -2015,7 +2015,7 @@
         <v>42690</v>
       </c>
       <c r="G66" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Added 2 Requirements, Added user stories #58-67
</commit_message>
<xml_diff>
--- a/Functional Requirements.xlsx
+++ b/Functional Requirements.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="75">
   <si>
     <t>ID</t>
   </si>
@@ -219,22 +219,28 @@
     <t>The list of all of the teachers in a specific class can be viewed</t>
   </si>
   <si>
-    <t>Teacher's details can be viewed be clicking on him</t>
-  </si>
-  <si>
-    <t>Pupil's details can be viewed by clicking on him</t>
-  </si>
-  <si>
-    <t>The list of all of the teachers can be viewed</t>
-  </si>
-  <si>
-    <t>The list of all of the pupils can be viewed</t>
-  </si>
-  <si>
     <t>Ability to answer questions related to a text after reading it</t>
   </si>
   <si>
     <t xml:space="preserve">"Check" button - upon clicking the pupil recieves feedback for answer  </t>
+  </si>
+  <si>
+    <t>Pupil's details can be viewed by any teacher teaching him</t>
+  </si>
+  <si>
+    <t>A list of all pupils in the system can be viewed</t>
+  </si>
+  <si>
+    <t>A list of al teachers in the system can be viewed</t>
+  </si>
+  <si>
+    <t>Pupil's details can be viewed by himself</t>
+  </si>
+  <si>
+    <t>Details about a teacher can be viewed by all teachers</t>
+  </si>
+  <si>
+    <t>Details about a teacher can be viewed by their pupils</t>
   </si>
 </sst>
 </file>
@@ -631,10 +637,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G71"/>
+  <dimension ref="A1:G72"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="B66" sqref="B66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -759,7 +765,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C6" s="3">
         <v>5</v>
@@ -1011,7 +1017,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C18" s="3">
         <v>5</v>
@@ -1943,7 +1949,7 @@
         <v>62</v>
       </c>
       <c r="B63" s="5" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C63" s="3">
         <v>5</v>
@@ -1952,7 +1958,7 @@
         <v>2</v>
       </c>
       <c r="E63" s="4">
-        <v>42690</v>
+        <v>42703</v>
       </c>
       <c r="G63" s="3" t="s">
         <v>53</v>
@@ -1963,7 +1969,7 @@
         <v>63</v>
       </c>
       <c r="B64" s="5" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="C64" s="3">
         <v>5</v>
@@ -1972,7 +1978,7 @@
         <v>2</v>
       </c>
       <c r="E64" s="4">
-        <v>42690</v>
+        <v>42703</v>
       </c>
       <c r="G64" s="3" t="s">
         <v>53</v>
@@ -1983,7 +1989,7 @@
         <v>64</v>
       </c>
       <c r="B65" s="5" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="C65" s="3">
         <v>5</v>
@@ -1992,7 +1998,7 @@
         <v>2</v>
       </c>
       <c r="E65" s="4">
-        <v>42690</v>
+        <v>42703</v>
       </c>
       <c r="G65" s="3" t="s">
         <v>53</v>
@@ -2003,7 +2009,7 @@
         <v>65</v>
       </c>
       <c r="B66" s="5" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C66" s="3">
         <v>5</v>
@@ -2012,7 +2018,7 @@
         <v>2</v>
       </c>
       <c r="E66" s="4">
-        <v>42690</v>
+        <v>42703</v>
       </c>
       <c r="G66" s="3" t="s">
         <v>53</v>
@@ -2022,11 +2028,41 @@
       <c r="A67" s="1">
         <v>66</v>
       </c>
+      <c r="B67" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C67" s="3">
+        <v>5</v>
+      </c>
+      <c r="D67" s="3">
+        <v>2</v>
+      </c>
+      <c r="E67" s="4">
+        <v>42690</v>
+      </c>
+      <c r="G67" s="3" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
         <v>67</v>
       </c>
+      <c r="B68" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C68" s="3">
+        <v>5</v>
+      </c>
+      <c r="D68" s="3">
+        <v>2</v>
+      </c>
+      <c r="E68" s="4">
+        <v>42690</v>
+      </c>
+      <c r="G68" s="3" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
@@ -2042,6 +2078,9 @@
       <c r="A71" s="1">
         <v>70</v>
       </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A72" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
UI improvements - SmartTextBox + TextView
</commit_message>
<xml_diff>
--- a/Functional Requirements.xlsx
+++ b/Functional Requirements.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="82">
   <si>
     <t>ID</t>
   </si>
@@ -688,7 +688,7 @@
   <dimension ref="A1:H72"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N22" sqref="N22"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -922,10 +922,12 @@
         <v>42686</v>
       </c>
       <c r="F10" s="3"/>
-      <c r="G10" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="H10" s="3"/>
+      <c r="G10" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1">

</xml_diff>

<commit_message>
SmartTextBox UI - viewing definitions of words
</commit_message>
<xml_diff>
--- a/Functional Requirements.xlsx
+++ b/Functional Requirements.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="82">
   <si>
     <t>ID</t>
   </si>
@@ -688,7 +688,7 @@
   <dimension ref="A1:H72"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -812,10 +812,12 @@
         <v>42686</v>
       </c>
       <c r="F5" s="3"/>
-      <c r="G5" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="H5" s="3"/>
+      <c r="G5" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1">

</xml_diff>

<commit_message>
teacher stuff in admin area
</commit_message>
<xml_diff>
--- a/Functional Requirements.xlsx
+++ b/Functional Requirements.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17927"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="81">
   <si>
     <t>ID</t>
   </si>
@@ -256,12 +256,15 @@
   </si>
   <si>
     <t>21/04/2017</t>
+  </si>
+  <si>
+    <t>Testing</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -392,7 +395,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -425,9 +428,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -460,6 +480,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -639,7 +676,7 @@
   <dimension ref="A1:H72"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="G65" sqref="G65"/>
+      <selection activeCell="G62" sqref="G62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1864,7 +1901,7 @@
         <v>42687</v>
       </c>
       <c r="G55" s="6" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="H55" s="3"/>
     </row>
@@ -1885,7 +1922,7 @@
         <v>42687</v>
       </c>
       <c r="G56" s="6" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="H56" s="3"/>
     </row>
@@ -1906,7 +1943,7 @@
         <v>42687</v>
       </c>
       <c r="G57" s="6" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="H57" s="3"/>
     </row>
@@ -1927,7 +1964,7 @@
         <v>42687</v>
       </c>
       <c r="G58" s="6" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="H58" s="3"/>
     </row>
@@ -1969,7 +2006,7 @@
         <v>42690</v>
       </c>
       <c r="G60" s="6" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="H60" s="3"/>
     </row>
@@ -1990,7 +2027,7 @@
         <v>42690</v>
       </c>
       <c r="G61" s="6" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="H61" s="3"/>
     </row>
@@ -2011,7 +2048,7 @@
         <v>42690</v>
       </c>
       <c r="G62" s="6" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="H62" s="3"/>
     </row>

</xml_diff>

<commit_message>
added integration tests project, working on more backend tests
</commit_message>
<xml_diff>
--- a/Functional Requirements.xlsx
+++ b/Functional Requirements.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="82">
   <si>
     <t>ID</t>
   </si>
@@ -259,6 +259,9 @@
   </si>
   <si>
     <t>Testing</t>
+  </si>
+  <si>
+    <t>Unit Tests</t>
   </si>
 </sst>
 </file>
@@ -673,10 +676,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H72"/>
+  <dimension ref="A1:I72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="G62" sqref="G62"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -686,10 +689,13 @@
     <col min="5" max="5" width="19.375" customWidth="1"/>
     <col min="6" max="6" width="16.875" customWidth="1"/>
     <col min="7" max="7" width="16.375" customWidth="1"/>
-    <col min="8" max="8" width="20.625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25" customWidth="1"/>
+    <col min="9" max="9" width="15.75" customWidth="1"/>
+    <col min="10" max="10" width="16" customWidth="1"/>
+    <col min="11" max="11" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -714,8 +720,11 @@
       <c r="H1" s="2" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I1" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -739,7 +748,7 @@
       </c>
       <c r="H2" s="3"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -761,7 +770,7 @@
       </c>
       <c r="H3" s="3"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -783,7 +792,7 @@
       </c>
       <c r="H4" s="3"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -809,7 +818,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -831,7 +840,7 @@
       </c>
       <c r="H6" s="3"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -855,7 +864,7 @@
       </c>
       <c r="H7" s="3"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -879,7 +888,7 @@
       </c>
       <c r="H8" s="3"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -903,7 +912,7 @@
       </c>
       <c r="H9" s="3"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -919,7 +928,9 @@
       <c r="E10" s="4">
         <v>42686</v>
       </c>
-      <c r="F10" s="3"/>
+      <c r="F10" s="3" t="s">
+        <v>79</v>
+      </c>
       <c r="G10" s="7" t="s">
         <v>74</v>
       </c>
@@ -927,7 +938,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -951,7 +962,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -975,7 +986,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -997,7 +1008,7 @@
       </c>
       <c r="H13" s="3"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -1019,7 +1030,7 @@
       </c>
       <c r="H14" s="3"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -1041,7 +1052,7 @@
       </c>
       <c r="H15" s="3"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -1171,7 +1182,9 @@
       <c r="E21" s="4">
         <v>42686</v>
       </c>
-      <c r="F21" s="3"/>
+      <c r="F21" s="3" t="s">
+        <v>79</v>
+      </c>
       <c r="G21" s="7" t="s">
         <v>74</v>
       </c>

</xml_diff>

<commit_message>
Tasks for last iteration
</commit_message>
<xml_diff>
--- a/Functional Requirements.xlsx
+++ b/Functional Requirements.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17927"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17329"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="86">
   <si>
     <t>ID</t>
   </si>
@@ -262,6 +262,18 @@
   </si>
   <si>
     <t>Unit Tests</t>
+  </si>
+  <si>
+    <t>14/05/2017</t>
+  </si>
+  <si>
+    <t>27/04/2017</t>
+  </si>
+  <si>
+    <t>20/01/2017</t>
+  </si>
+  <si>
+    <t>New</t>
   </si>
 </sst>
 </file>
@@ -272,7 +284,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -280,12 +292,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -304,6 +316,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -317,7 +335,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -336,6 +354,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -678,24 +699,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I72"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F37" sqref="F37"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="J45" sqref="J45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="56.375" customWidth="1"/>
-    <col min="4" max="4" width="11.625" customWidth="1"/>
-    <col min="5" max="5" width="19.375" customWidth="1"/>
-    <col min="6" max="6" width="16.875" customWidth="1"/>
-    <col min="7" max="7" width="16.375" customWidth="1"/>
+    <col min="2" max="2" width="56.42578125" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" customWidth="1"/>
+    <col min="5" max="5" width="19.42578125" customWidth="1"/>
+    <col min="6" max="6" width="16.85546875" customWidth="1"/>
+    <col min="7" max="7" width="16.42578125" customWidth="1"/>
     <col min="8" max="8" width="25" customWidth="1"/>
-    <col min="9" max="9" width="15.75" customWidth="1"/>
+    <col min="9" max="9" width="15.7109375" customWidth="1"/>
     <col min="10" max="10" width="16" customWidth="1"/>
     <col min="11" max="11" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -724,7 +745,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -748,7 +769,7 @@
       </c>
       <c r="H2" s="3"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -770,7 +791,7 @@
       </c>
       <c r="H3" s="3"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -792,7 +813,7 @@
       </c>
       <c r="H4" s="3"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -808,17 +829,15 @@
       <c r="E5" s="4">
         <v>42686</v>
       </c>
-      <c r="F5" s="4">
-        <v>42852</v>
+      <c r="F5" s="4" t="s">
+        <v>83</v>
       </c>
       <c r="G5" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="H5" s="3" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H5" s="3"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -834,13 +853,15 @@
       <c r="E6" s="4">
         <v>42686</v>
       </c>
-      <c r="F6" s="3"/>
-      <c r="G6" s="6" t="s">
-        <v>72</v>
+      <c r="F6" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>74</v>
       </c>
       <c r="H6" s="3"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -857,14 +878,14 @@
         <v>42686</v>
       </c>
       <c r="F7" s="4">
-        <v>42804</v>
+        <v>43011</v>
       </c>
       <c r="G7" s="7" t="s">
         <v>74</v>
       </c>
       <c r="H7" s="3"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -881,14 +902,14 @@
         <v>42686</v>
       </c>
       <c r="F8" s="4">
-        <v>42804</v>
+        <v>43011</v>
       </c>
       <c r="G8" s="7" t="s">
         <v>74</v>
       </c>
       <c r="H8" s="3"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -905,14 +926,14 @@
         <v>42686</v>
       </c>
       <c r="F9" s="4">
-        <v>42804</v>
+        <v>43011</v>
       </c>
       <c r="G9" s="7" t="s">
         <v>74</v>
       </c>
       <c r="H9" s="3"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -934,11 +955,9 @@
       <c r="G10" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="H10" s="3" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H10" s="3"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -955,14 +974,14 @@
         <v>42686</v>
       </c>
       <c r="F11" s="3"/>
-      <c r="G11" s="7" t="s">
-        <v>74</v>
+      <c r="G11" s="6" t="s">
+        <v>72</v>
       </c>
       <c r="H11" s="3" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -979,14 +998,14 @@
         <v>42686</v>
       </c>
       <c r="F12" s="3"/>
-      <c r="G12" s="7" t="s">
-        <v>74</v>
+      <c r="G12" s="6" t="s">
+        <v>72</v>
       </c>
       <c r="H12" s="3" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -1008,7 +1027,7 @@
       </c>
       <c r="H13" s="3"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -1025,12 +1044,12 @@
         <v>42686</v>
       </c>
       <c r="F14" s="3"/>
-      <c r="G14" s="6" t="s">
-        <v>72</v>
+      <c r="G14" s="8" t="s">
+        <v>85</v>
       </c>
       <c r="H14" s="3"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -1047,12 +1066,12 @@
         <v>42686</v>
       </c>
       <c r="F15" s="3"/>
-      <c r="G15" s="6" t="s">
-        <v>72</v>
+      <c r="G15" s="8" t="s">
+        <v>85</v>
       </c>
       <c r="H15" s="3"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -1074,7 +1093,7 @@
       </c>
       <c r="H16" s="3"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -1091,12 +1110,12 @@
         <v>42686</v>
       </c>
       <c r="F17" s="3"/>
-      <c r="G17" s="6" t="s">
-        <v>72</v>
+      <c r="G17" s="8" t="s">
+        <v>85</v>
       </c>
       <c r="H17" s="3"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -1112,15 +1131,15 @@
       <c r="E18" s="4">
         <v>42686</v>
       </c>
-      <c r="F18" s="4">
-        <v>42755</v>
+      <c r="F18" s="4" t="s">
+        <v>84</v>
       </c>
       <c r="G18" s="7" t="s">
         <v>74</v>
       </c>
       <c r="H18" s="3"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -1142,7 +1161,7 @@
       </c>
       <c r="H19" s="3"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -1166,7 +1185,7 @@
       </c>
       <c r="H20" s="3"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -1190,7 +1209,7 @@
       </c>
       <c r="H21" s="3"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -1214,7 +1233,7 @@
       </c>
       <c r="H22" s="3"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -1231,12 +1250,12 @@
         <v>42686</v>
       </c>
       <c r="F23" s="3"/>
-      <c r="G23" s="6" t="s">
-        <v>72</v>
+      <c r="G23" s="8" t="s">
+        <v>85</v>
       </c>
       <c r="H23" s="3"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -1253,12 +1272,12 @@
         <v>42686</v>
       </c>
       <c r="F24" s="3"/>
-      <c r="G24" s="6" t="s">
-        <v>72</v>
+      <c r="G24" s="8" t="s">
+        <v>85</v>
       </c>
       <c r="H24" s="3"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -1275,12 +1294,12 @@
         <v>42686</v>
       </c>
       <c r="F25" s="3"/>
-      <c r="G25" s="6" t="s">
-        <v>72</v>
+      <c r="G25" s="8" t="s">
+        <v>85</v>
       </c>
       <c r="H25" s="3"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -1304,7 +1323,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -1326,7 +1345,7 @@
       </c>
       <c r="H27" s="3"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -1348,7 +1367,7 @@
       </c>
       <c r="H28" s="3"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -1365,14 +1384,12 @@
         <v>42686</v>
       </c>
       <c r="F29" s="3"/>
-      <c r="G29" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="H29" s="3" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G29" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="H29" s="3"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -1394,7 +1411,7 @@
       </c>
       <c r="H30" s="3"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -1416,7 +1433,7 @@
       </c>
       <c r="H31" s="3"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -1436,11 +1453,9 @@
       <c r="G32" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="H32" s="3" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H32" s="3"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>32</v>
       </c>
@@ -1462,7 +1477,7 @@
       </c>
       <c r="H33" s="3"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>33</v>
       </c>
@@ -1484,7 +1499,7 @@
       </c>
       <c r="H34" s="3"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>34</v>
       </c>
@@ -1506,7 +1521,7 @@
       </c>
       <c r="H35" s="3"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>35</v>
       </c>
@@ -1528,7 +1543,7 @@
       </c>
       <c r="H36" s="3"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>36</v>
       </c>
@@ -1552,7 +1567,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>37</v>
       </c>
@@ -1574,7 +1589,7 @@
       </c>
       <c r="H38" s="3"/>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>38</v>
       </c>
@@ -1596,7 +1611,7 @@
       </c>
       <c r="H39" s="3"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>39</v>
       </c>
@@ -1618,7 +1633,7 @@
       </c>
       <c r="H40" s="3"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>40</v>
       </c>
@@ -1640,7 +1655,7 @@
       </c>
       <c r="H41" s="3"/>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>41</v>
       </c>
@@ -1662,7 +1677,7 @@
       </c>
       <c r="H42" s="3"/>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>42</v>
       </c>
@@ -1684,7 +1699,7 @@
       </c>
       <c r="H43" s="3"/>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>43</v>
       </c>
@@ -1694,7 +1709,7 @@
       <c r="F44" s="3"/>
       <c r="H44" s="3"/>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="C45" s="3"/>
       <c r="D45" s="3"/>
@@ -1702,7 +1717,7 @@
       <c r="F45" s="3"/>
       <c r="H45" s="3"/>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>45</v>
       </c>
@@ -1724,7 +1739,7 @@
       </c>
       <c r="H46" s="3"/>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>46</v>
       </c>
@@ -1746,7 +1761,7 @@
       </c>
       <c r="H47" s="3"/>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>47</v>
       </c>
@@ -1768,7 +1783,7 @@
       </c>
       <c r="H48" s="3"/>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>48</v>
       </c>
@@ -1790,7 +1805,7 @@
       </c>
       <c r="H49" s="3"/>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>49</v>
       </c>
@@ -1813,7 +1828,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>50</v>
       </c>
@@ -1834,7 +1849,7 @@
       </c>
       <c r="H51" s="3"/>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>51</v>
       </c>
@@ -1855,7 +1870,7 @@
       </c>
       <c r="H52" s="3"/>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>52</v>
       </c>
@@ -1876,7 +1891,7 @@
       </c>
       <c r="H53" s="3"/>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>53</v>
       </c>
@@ -1897,7 +1912,7 @@
       </c>
       <c r="H54" s="3"/>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>54</v>
       </c>
@@ -1918,7 +1933,7 @@
       </c>
       <c r="H55" s="3"/>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>55</v>
       </c>
@@ -1939,7 +1954,7 @@
       </c>
       <c r="H56" s="3"/>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>56</v>
       </c>
@@ -1960,7 +1975,7 @@
       </c>
       <c r="H57" s="3"/>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>57</v>
       </c>
@@ -1981,7 +1996,7 @@
       </c>
       <c r="H58" s="3"/>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>58</v>
       </c>
@@ -2002,7 +2017,7 @@
       </c>
       <c r="H59" s="3"/>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>59</v>
       </c>
@@ -2023,7 +2038,7 @@
       </c>
       <c r="H60" s="3"/>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>60</v>
       </c>
@@ -2044,7 +2059,7 @@
       </c>
       <c r="H61" s="3"/>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>61</v>
       </c>
@@ -2065,7 +2080,7 @@
       </c>
       <c r="H62" s="3"/>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>62</v>
       </c>
@@ -2086,7 +2101,7 @@
       </c>
       <c r="H63" s="3"/>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>63</v>
       </c>
@@ -2107,7 +2122,7 @@
       </c>
       <c r="H64" s="3"/>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>64</v>
       </c>
@@ -2128,7 +2143,7 @@
       </c>
       <c r="H65" s="3"/>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>65</v>
       </c>
@@ -2149,7 +2164,7 @@
       </c>
       <c r="H66" s="3"/>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>66</v>
       </c>
@@ -2170,7 +2185,7 @@
       </c>
       <c r="H67" s="3"/>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>67</v>
       </c>
@@ -2191,16 +2206,16 @@
       </c>
       <c r="H68" s="3"/>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="1"/>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="1"/>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="1"/>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="1"/>
     </row>
   </sheetData>
@@ -2217,7 +2232,7 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2229,7 +2244,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Functional Requirements + Tasks update
</commit_message>
<xml_diff>
--- a/Functional Requirements.xlsx
+++ b/Functional Requirements.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="89">
   <si>
     <t>ID</t>
   </si>
@@ -280,6 +280,9 @@
   </si>
   <si>
     <t>27/05/2017</t>
+  </si>
+  <si>
+    <t>28/05/2017</t>
   </si>
 </sst>
 </file>
@@ -705,8 +708,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="H48" sqref="H48"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H65" sqref="H65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1547,9 +1550,11 @@
       <c r="E36" s="4">
         <v>42686</v>
       </c>
-      <c r="F36" s="3"/>
-      <c r="G36" s="6" t="s">
-        <v>72</v>
+      <c r="F36" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="G36" s="7" t="s">
+        <v>74</v>
       </c>
       <c r="H36" s="3"/>
     </row>
@@ -2119,8 +2124,11 @@
       <c r="E61" s="4">
         <v>42703</v>
       </c>
-      <c r="G61" s="6" t="s">
-        <v>72</v>
+      <c r="F61" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="G61" s="7" t="s">
+        <v>74</v>
       </c>
       <c r="H61" s="3"/>
     </row>
@@ -2224,8 +2232,11 @@
       <c r="E66" s="4">
         <v>42690</v>
       </c>
-      <c r="G66" s="6" t="s">
-        <v>72</v>
+      <c r="F66" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="G66" s="7" t="s">
+        <v>74</v>
       </c>
       <c r="H66" s="3"/>
     </row>

</xml_diff>

<commit_message>
word definition tests for full traceability +started tracing
</commit_message>
<xml_diff>
--- a/Functional Requirements.xlsx
+++ b/Functional Requirements.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17329"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18067"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="91">
   <si>
     <t>ID</t>
   </si>
@@ -261,9 +261,6 @@
     <t>Testing</t>
   </si>
   <si>
-    <t>Unit Tests</t>
-  </si>
-  <si>
     <t>14/05/2017</t>
   </si>
   <si>
@@ -283,6 +280,15 @@
   </si>
   <si>
     <t>28/05/2017</t>
+  </si>
+  <si>
+    <t>Tests</t>
+  </si>
+  <si>
+    <t>AS1-5,AS9-10,AR1,AR3,DER1,DER3</t>
+  </si>
+  <si>
+    <t>TS4-7,TR2-3,TR6-7</t>
   </si>
 </sst>
 </file>
@@ -293,7 +299,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -301,7 +307,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -709,23 +715,23 @@
   <dimension ref="A1:I72"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H65" sqref="H65"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="56.42578125" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" customWidth="1"/>
-    <col min="5" max="5" width="19.42578125" customWidth="1"/>
-    <col min="6" max="6" width="16.85546875" customWidth="1"/>
-    <col min="7" max="7" width="16.42578125" customWidth="1"/>
+    <col min="2" max="2" width="56.375" customWidth="1"/>
+    <col min="4" max="4" width="11.625" customWidth="1"/>
+    <col min="5" max="5" width="19.375" customWidth="1"/>
+    <col min="6" max="6" width="16.875" customWidth="1"/>
+    <col min="7" max="7" width="16.375" customWidth="1"/>
     <col min="8" max="8" width="25" customWidth="1"/>
-    <col min="9" max="9" width="15.7109375" customWidth="1"/>
+    <col min="9" max="9" width="44.375" customWidth="1"/>
     <col min="10" max="10" width="16" customWidth="1"/>
     <col min="11" max="11" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -751,10 +757,10 @@
         <v>73</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -777,8 +783,11 @@
         <v>74</v>
       </c>
       <c r="H2" s="3"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -800,7 +809,7 @@
       </c>
       <c r="H3" s="3"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -822,7 +831,7 @@
       </c>
       <c r="H4" s="3"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -839,14 +848,14 @@
         <v>42686</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G5" s="7" t="s">
         <v>74</v>
       </c>
       <c r="H5" s="3"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -863,14 +872,17 @@
         <v>42686</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G6" s="7" t="s">
         <v>74</v>
       </c>
       <c r="H6" s="3"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I6" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -894,7 +906,7 @@
       </c>
       <c r="H7" s="3"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -918,7 +930,7 @@
       </c>
       <c r="H8" s="3"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -942,7 +954,7 @@
       </c>
       <c r="H9" s="3"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -966,7 +978,7 @@
       </c>
       <c r="H10" s="3"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -990,7 +1002,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -1014,7 +1026,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -1036,7 +1048,7 @@
       </c>
       <c r="H13" s="3"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -1054,11 +1066,11 @@
       </c>
       <c r="F14" s="3"/>
       <c r="G14" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H14" s="3"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -1076,11 +1088,11 @@
       </c>
       <c r="F15" s="3"/>
       <c r="G15" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H15" s="3"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -1102,7 +1114,7 @@
       </c>
       <c r="H16" s="3"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -1120,11 +1132,11 @@
       </c>
       <c r="F17" s="3"/>
       <c r="G17" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H17" s="3"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -1141,14 +1153,14 @@
         <v>42686</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G18" s="7" t="s">
         <v>74</v>
       </c>
       <c r="H18" s="3"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -1170,7 +1182,7 @@
       </c>
       <c r="H19" s="3"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -1194,7 +1206,7 @@
       </c>
       <c r="H20" s="3"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -1218,7 +1230,7 @@
       </c>
       <c r="H21" s="3"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -1242,7 +1254,7 @@
       </c>
       <c r="H22" s="3"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -1260,11 +1272,11 @@
       </c>
       <c r="F23" s="3"/>
       <c r="G23" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H23" s="3"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -1282,11 +1294,11 @@
       </c>
       <c r="F24" s="3"/>
       <c r="G24" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H24" s="3"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -1304,11 +1316,11 @@
       </c>
       <c r="F25" s="3"/>
       <c r="G25" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H25" s="3"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -1325,14 +1337,14 @@
         <v>42686</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G26" s="7" t="s">
         <v>74</v>
       </c>
       <c r="H26" s="3"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -1350,11 +1362,11 @@
       </c>
       <c r="F27" s="3"/>
       <c r="G27" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H27" s="3"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -1372,11 +1384,11 @@
       </c>
       <c r="F28" s="3"/>
       <c r="G28" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H28" s="3"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -1393,14 +1405,14 @@
         <v>42686</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G29" s="7" t="s">
         <v>74</v>
       </c>
       <c r="H29" s="3"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -1418,11 +1430,11 @@
       </c>
       <c r="F30" s="3"/>
       <c r="G30" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H30" s="3"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -1440,11 +1452,11 @@
       </c>
       <c r="F31" s="3"/>
       <c r="G31" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H31" s="3"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -1461,14 +1473,14 @@
         <v>42686</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G32" s="7" t="s">
         <v>74</v>
       </c>
       <c r="H32" s="3"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>32</v>
       </c>
@@ -1486,11 +1498,11 @@
       </c>
       <c r="F33" s="3"/>
       <c r="G33" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H33" s="3"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>33</v>
       </c>
@@ -1508,11 +1520,11 @@
       </c>
       <c r="F34" s="3"/>
       <c r="G34" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H34" s="3"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>34</v>
       </c>
@@ -1534,7 +1546,7 @@
       </c>
       <c r="H35" s="3"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>35</v>
       </c>
@@ -1551,14 +1563,14 @@
         <v>42686</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G36" s="7" t="s">
         <v>74</v>
       </c>
       <c r="H36" s="3"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>36</v>
       </c>
@@ -1575,7 +1587,7 @@
         <v>42686</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G37" s="7" t="s">
         <v>74</v>
@@ -1584,7 +1596,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>37</v>
       </c>
@@ -1601,14 +1613,14 @@
         <v>42686</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G38" s="7" t="s">
         <v>74</v>
       </c>
       <c r="H38" s="3"/>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>38</v>
       </c>
@@ -1625,14 +1637,14 @@
         <v>42686</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G39" s="7" t="s">
         <v>74</v>
       </c>
       <c r="H39" s="3"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>39</v>
       </c>
@@ -1649,14 +1661,14 @@
         <v>42686</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G40" s="7" t="s">
         <v>74</v>
       </c>
       <c r="H40" s="3"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>40</v>
       </c>
@@ -1673,14 +1685,14 @@
         <v>42686</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G41" s="7" t="s">
         <v>74</v>
       </c>
       <c r="H41" s="3"/>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>41</v>
       </c>
@@ -1697,14 +1709,14 @@
         <v>42686</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G42" s="7" t="s">
         <v>74</v>
       </c>
       <c r="H42" s="3"/>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>42</v>
       </c>
@@ -1721,14 +1733,14 @@
         <v>42686</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G43" s="7" t="s">
         <v>74</v>
       </c>
       <c r="H43" s="3"/>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>43</v>
       </c>
@@ -1745,14 +1757,14 @@
         <v>42686</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G44" s="7" t="s">
         <v>74</v>
       </c>
       <c r="H44" s="3"/>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>44</v>
       </c>
@@ -1769,14 +1781,14 @@
         <v>42686</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G45" s="7" t="s">
         <v>74</v>
       </c>
       <c r="H45" s="3"/>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>45</v>
       </c>
@@ -1793,14 +1805,14 @@
         <v>42686</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G46" s="7" t="s">
         <v>74</v>
       </c>
       <c r="H46" s="3"/>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>46</v>
       </c>
@@ -1817,14 +1829,14 @@
         <v>42686</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G47" s="7" t="s">
         <v>74</v>
       </c>
       <c r="H47" s="3"/>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>47</v>
       </c>
@@ -1847,7 +1859,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>48</v>
       </c>
@@ -1868,7 +1880,7 @@
       </c>
       <c r="H49" s="3"/>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>49</v>
       </c>
@@ -1885,14 +1897,14 @@
         <v>42687</v>
       </c>
       <c r="F50" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G50" s="7" t="s">
         <v>74</v>
       </c>
       <c r="H50" s="3"/>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>50</v>
       </c>
@@ -1909,14 +1921,14 @@
         <v>42687</v>
       </c>
       <c r="F51" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G51" s="7" t="s">
         <v>74</v>
       </c>
       <c r="H51" s="3"/>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>51</v>
       </c>
@@ -1933,14 +1945,14 @@
         <v>42687</v>
       </c>
       <c r="F52" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G52" s="7" t="s">
         <v>74</v>
       </c>
       <c r="H52" s="3"/>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
         <v>52</v>
       </c>
@@ -1961,7 +1973,7 @@
       </c>
       <c r="H53" s="3"/>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
         <v>53</v>
       </c>
@@ -1982,7 +1994,7 @@
       </c>
       <c r="H54" s="3"/>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
         <v>54</v>
       </c>
@@ -2003,7 +2015,7 @@
       </c>
       <c r="H55" s="3"/>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
         <v>55</v>
       </c>
@@ -2024,7 +2036,7 @@
       </c>
       <c r="H56" s="3"/>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
         <v>56</v>
       </c>
@@ -2045,7 +2057,7 @@
       </c>
       <c r="H57" s="3"/>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
         <v>57</v>
       </c>
@@ -2066,7 +2078,7 @@
       </c>
       <c r="H58" s="3"/>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
         <v>58</v>
       </c>
@@ -2087,7 +2099,7 @@
       </c>
       <c r="H59" s="3"/>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
         <v>59</v>
       </c>
@@ -2108,7 +2120,7 @@
       </c>
       <c r="H60" s="3"/>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
         <v>60</v>
       </c>
@@ -2125,14 +2137,14 @@
         <v>42703</v>
       </c>
       <c r="F61" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G61" s="7" t="s">
         <v>74</v>
       </c>
       <c r="H61" s="3"/>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
         <v>61</v>
       </c>
@@ -2153,7 +2165,7 @@
       </c>
       <c r="H62" s="3"/>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
         <v>62</v>
       </c>
@@ -2174,7 +2186,7 @@
       </c>
       <c r="H63" s="3"/>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
         <v>63</v>
       </c>
@@ -2195,7 +2207,7 @@
       </c>
       <c r="H64" s="3"/>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
         <v>64</v>
       </c>
@@ -2216,7 +2228,7 @@
       </c>
       <c r="H65" s="3"/>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
         <v>65</v>
       </c>
@@ -2233,23 +2245,23 @@
         <v>42690</v>
       </c>
       <c r="F66" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G66" s="7" t="s">
         <v>74</v>
       </c>
       <c r="H66" s="3"/>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A69" s="1"/>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A70" s="1"/>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A71" s="1"/>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A72" s="1"/>
     </row>
   </sheetData>
@@ -2266,7 +2278,7 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2278,7 +2290,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
almost done with Tracing
</commit_message>
<xml_diff>
--- a/Functional Requirements.xlsx
+++ b/Functional Requirements.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="119">
   <si>
     <t>ID</t>
   </si>
@@ -346,6 +346,33 @@
   </si>
   <si>
     <t>Answer could be submitted</t>
+  </si>
+  <si>
+    <t>AS10.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SCS13.2, SCS12.3, SCR4,DER3 </t>
+  </si>
+  <si>
+    <t>SCS13.1,SCS12.3,SCR4,DER3</t>
+  </si>
+  <si>
+    <t>SCS13.4,SCS12.3,SCR3,DER3</t>
+  </si>
+  <si>
+    <t>SCS1-3,SCR1,DER1</t>
+  </si>
+  <si>
+    <t>SCS10-13.5,SCR4,DER3</t>
+  </si>
+  <si>
+    <t>SCS14-19,SCR5,DER4</t>
+  </si>
+  <si>
+    <t>SCS13.5,SCR4,DER3</t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
 </sst>
 </file>
@@ -806,8 +833,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B51" sqref="B51"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="I61" sqref="I61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2007,8 +2034,11 @@
       <c r="H48" s="3" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I48" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>48</v>
       </c>
@@ -2031,8 +2061,11 @@
         <v>73</v>
       </c>
       <c r="H49" s="3"/>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I49" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>49</v>
       </c>
@@ -2055,8 +2088,11 @@
         <v>73</v>
       </c>
       <c r="H50" s="3"/>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I50" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>50</v>
       </c>
@@ -2079,8 +2115,11 @@
         <v>73</v>
       </c>
       <c r="H51" s="3"/>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I51" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>51</v>
       </c>
@@ -2103,8 +2142,11 @@
         <v>73</v>
       </c>
       <c r="H52" s="3"/>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I52" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
         <v>52</v>
       </c>
@@ -2124,8 +2166,11 @@
         <v>79</v>
       </c>
       <c r="H53" s="3"/>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I53" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
         <v>53</v>
       </c>
@@ -2145,8 +2190,11 @@
         <v>79</v>
       </c>
       <c r="H54" s="3"/>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I54" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
         <v>54</v>
       </c>
@@ -2166,8 +2214,11 @@
         <v>79</v>
       </c>
       <c r="H55" s="3"/>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I55" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
         <v>55</v>
       </c>
@@ -2187,8 +2238,11 @@
         <v>79</v>
       </c>
       <c r="H56" s="3"/>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I56" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
         <v>56</v>
       </c>
@@ -2209,7 +2263,7 @@
       </c>
       <c r="H57" s="3"/>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
         <v>57</v>
       </c>
@@ -2229,8 +2283,11 @@
         <v>79</v>
       </c>
       <c r="H58" s="3"/>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I58" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
         <v>58</v>
       </c>
@@ -2250,8 +2307,11 @@
         <v>79</v>
       </c>
       <c r="H59" s="3"/>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I59" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
         <v>59</v>
       </c>
@@ -2271,8 +2331,11 @@
         <v>79</v>
       </c>
       <c r="H60" s="3"/>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I60" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
         <v>60</v>
       </c>
@@ -2296,7 +2359,7 @@
       </c>
       <c r="H61" s="3"/>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
         <v>61</v>
       </c>
@@ -2317,7 +2380,7 @@
       </c>
       <c r="H62" s="3"/>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
         <v>62</v>
       </c>
@@ -2338,7 +2401,7 @@
       </c>
       <c r="H63" s="3"/>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
         <v>63</v>
       </c>

</xml_diff>